<commit_message>
verigen create_project template 수정
</commit_message>
<xml_diff>
--- a/Common/bin/project_template_verigen/verigen_src/config.xlsx
+++ b/Common/bin/project_template_verigen/verigen_src/config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Profiles\Common\bin\project_template_verigen\verigen_src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9911D36D-0954-452F-9759-66DC9CA6A319}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCC754BD-5A92-4184-8E13-14CA3409870F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="configuration" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Value</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -47,10 +47,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>MAXI bus data width</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>CLK_SPEED</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -59,15 +55,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Memory Block Size</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Common memory address width (32 ~ 64 bit)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Total multi-core count (1~)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* Processor configuration</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -78,7 +74,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="#,##0_ "/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -96,6 +92,16 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="15"/>
       <color theme="1"/>
       <name val="맑은 고딕"/>
       <family val="3"/>
@@ -144,7 +150,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -159,6 +165,7 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -439,11 +446,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
@@ -455,109 +460,77 @@
     <col min="7" max="7" width="19.5" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>8</v>
+    <row r="1" spans="1:7" ht="24" x14ac:dyDescent="0.45">
+      <c r="A1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="2">
+        <v>8192</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="5">
-        <v>4</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="2">
-        <v>128</v>
-      </c>
       <c r="G2" s="2">
-        <v>64</v>
+        <v>16384</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="5">
-        <v>36</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="2">
-        <v>256</v>
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="G3" s="2">
-        <v>128</v>
+        <v>32768</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B4" s="5">
-        <v>500</v>
+        <v>4</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G4" s="2">
-        <v>256</v>
+        <v>65536</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="G5" s="2">
-        <v>2048</v>
+      <c r="A5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5">
+        <v>36</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="G6" s="2">
-        <v>4096</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="G7" s="2">
-        <v>8192</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="G8" s="2">
-        <v>16384</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="G9" s="2">
-        <v>32768</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="G10" s="2">
-        <v>65536</v>
+      <c r="A6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5">
+        <v>500</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{0F04BC87-1C45-4F59-85DD-C10A788D5508}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{0F04BC87-1C45-4F59-85DD-C10A788D5508}">
       <formula1>32</formula1>
       <formula2>64</formula2>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{26DC951F-A9DD-4395-BF8B-05D3E8220847}">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4" xr:uid="{26DC951F-A9DD-4395-BF8B-05D3E8220847}">
       <formula1>1</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>